<commit_message>
march 3 2023 update
</commit_message>
<xml_diff>
--- a/db/uploads/EMPLOYEE-MASTERLIST.xlsx
+++ b/db/uploads/EMPLOYEE-MASTERLIST.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaysonregalario/Desktop/project/FranchisingCoop/db/uploads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaysonregalario/Desktop/project/test_gyrt/db/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014BDEB9-D605-D548-94B7-A426B944B9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AC82E5-FC33-9F4E-86AB-06C7C13E1D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29280" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29280" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$164</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$136</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="622">
   <si>
     <t>Employee no.</t>
   </si>
@@ -1890,13 +1890,28 @@
   </si>
   <si>
     <t>RAÑOA</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>EMP10201</t>
+  </si>
+  <si>
+    <t>ORETA</t>
+  </si>
+  <si>
+    <t>KATRINA</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1925,6 +1940,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1948,14 +1969,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2236,22 +2259,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="132" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="24.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="34" style="4" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="5" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2273,8 +2294,11 @@
       <c r="G1" s="1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2297,8 +2321,11 @@
       <c r="G2" s="3" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -2321,8 +2348,11 @@
       <c r="G3" s="3" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -2345,8 +2375,11 @@
       <c r="G4" s="3" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -2369,8 +2402,11 @@
       <c r="G5" s="3" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -2393,8 +2429,11 @@
       <c r="G6" s="3" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -2417,8 +2456,11 @@
       <c r="G7" s="3" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -2441,8 +2483,11 @@
       <c r="G8" s="3" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -2465,8 +2510,11 @@
       <c r="G9" s="3" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
@@ -2489,8 +2537,11 @@
       <c r="G10" s="3" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
@@ -2513,8 +2564,11 @@
       <c r="G11" s="3" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -2537,8 +2591,11 @@
       <c r="G12" s="3" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
@@ -2561,8 +2618,11 @@
       <c r="G13" s="3" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -2585,8 +2645,11 @@
       <c r="G14" s="3" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
@@ -2609,8 +2672,11 @@
       <c r="G15" s="3" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>59</v>
       </c>
@@ -2633,8 +2699,11 @@
       <c r="G16" s="3" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
@@ -2657,8 +2726,11 @@
       <c r="G17" s="3" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
@@ -2681,8 +2753,11 @@
       <c r="G18" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>71</v>
       </c>
@@ -2705,8 +2780,11 @@
       <c r="G19" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>75</v>
       </c>
@@ -2729,8 +2807,11 @@
       <c r="G20" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>79</v>
       </c>
@@ -2753,8 +2834,11 @@
       <c r="G21" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>83</v>
       </c>
@@ -2777,8 +2861,11 @@
       <c r="G22" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>87</v>
       </c>
@@ -2801,8 +2888,11 @@
       <c r="G23" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>91</v>
       </c>
@@ -2825,8 +2915,11 @@
       <c r="G24" s="3" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>95</v>
       </c>
@@ -2849,8 +2942,11 @@
       <c r="G25" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
@@ -2873,8 +2969,11 @@
       <c r="G26" s="3" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>103</v>
       </c>
@@ -2897,8 +2996,11 @@
       <c r="G27" s="3" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>107</v>
       </c>
@@ -2921,8 +3023,11 @@
       <c r="G28" s="3" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>111</v>
       </c>
@@ -2945,8 +3050,11 @@
       <c r="G29" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>115</v>
       </c>
@@ -2969,8 +3077,11 @@
       <c r="G30" s="3" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>119</v>
       </c>
@@ -2993,8 +3104,11 @@
       <c r="G31" s="3" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>123</v>
       </c>
@@ -3017,8 +3131,11 @@
       <c r="G32" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>127</v>
       </c>
@@ -3041,8 +3158,11 @@
       <c r="G33" s="3" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>131</v>
       </c>
@@ -3065,8 +3185,11 @@
       <c r="G34" s="3" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>135</v>
       </c>
@@ -3089,8 +3212,11 @@
       <c r="G35" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>139</v>
       </c>
@@ -3113,8 +3239,11 @@
       <c r="G36" s="3" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>142</v>
       </c>
@@ -3137,8 +3266,11 @@
       <c r="G37" s="3" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>146</v>
       </c>
@@ -3161,8 +3293,11 @@
       <c r="G38" s="3" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>150</v>
       </c>
@@ -3185,8 +3320,11 @@
       <c r="G39" s="3" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>154</v>
       </c>
@@ -3209,8 +3347,11 @@
       <c r="G40" s="3" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>157</v>
       </c>
@@ -3233,8 +3374,11 @@
       <c r="G41" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>161</v>
       </c>
@@ -3257,8 +3401,11 @@
       <c r="G42" s="3" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>165</v>
       </c>
@@ -3276,13 +3423,16 @@
         <v>Non-Life Division</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>169</v>
       </c>
@@ -3305,8 +3455,11 @@
       <c r="G44" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>173</v>
       </c>
@@ -3329,8 +3482,11 @@
       <c r="G45" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>177</v>
       </c>
@@ -3353,8 +3509,11 @@
       <c r="G46" s="3" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>181</v>
       </c>
@@ -3377,8 +3536,11 @@
       <c r="G47" s="3" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>185</v>
       </c>
@@ -3401,8 +3563,11 @@
       <c r="G48" s="3" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>189</v>
       </c>
@@ -3425,8 +3590,11 @@
       <c r="G49" s="3" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>193</v>
       </c>
@@ -3449,8 +3617,11 @@
       <c r="G50" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>197</v>
       </c>
@@ -3473,8 +3644,11 @@
       <c r="G51" s="3" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>201</v>
       </c>
@@ -3497,8 +3671,11 @@
       <c r="G52" s="3" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>206</v>
       </c>
@@ -3521,8 +3698,11 @@
       <c r="G53" s="3" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>210</v>
       </c>
@@ -3545,8 +3725,11 @@
       <c r="G54" s="3" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>214</v>
       </c>
@@ -3569,8 +3752,11 @@
       <c r="G55" s="3" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>218</v>
       </c>
@@ -3593,8 +3779,11 @@
       <c r="G56" s="3" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>222</v>
       </c>
@@ -3617,8 +3806,11 @@
       <c r="G57" s="3" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>226</v>
       </c>
@@ -3641,8 +3833,11 @@
       <c r="G58" s="3" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>230</v>
       </c>
@@ -3660,13 +3855,16 @@
         <v>Non-Life Division</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>234</v>
       </c>
@@ -3684,13 +3882,16 @@
         <v>Non-Life Division</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>238</v>
       </c>
@@ -3708,13 +3909,16 @@
         <v>Non-Life Division</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>242</v>
       </c>
@@ -3737,8 +3941,11 @@
       <c r="G62" s="3" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>246</v>
       </c>
@@ -3761,8 +3968,11 @@
       <c r="G63" s="3" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>249</v>
       </c>
@@ -3785,8 +3995,11 @@
       <c r="G64" s="3" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>253</v>
       </c>
@@ -3809,8 +4022,11 @@
       <c r="G65" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>257</v>
       </c>
@@ -3833,8 +4049,11 @@
       <c r="G66" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>261</v>
       </c>
@@ -3857,8 +4076,11 @@
       <c r="G67" s="3" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>265</v>
       </c>
@@ -3881,8 +4103,11 @@
       <c r="G68" s="3" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>268</v>
       </c>
@@ -3905,8 +4130,11 @@
       <c r="G69" s="3" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>272</v>
       </c>
@@ -3929,8 +4157,11 @@
       <c r="G70" s="3" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>276</v>
       </c>
@@ -3953,8 +4184,11 @@
       <c r="G71" s="3" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>280</v>
       </c>
@@ -3977,8 +4211,11 @@
       <c r="G72" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>284</v>
       </c>
@@ -4001,8 +4238,11 @@
       <c r="G73" s="3" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>287</v>
       </c>
@@ -4020,13 +4260,16 @@
         <v>Non-Life Division</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>290</v>
       </c>
@@ -4049,8 +4292,11 @@
       <c r="G75" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>294</v>
       </c>
@@ -4073,8 +4319,11 @@
       <c r="G76" s="3" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>299</v>
       </c>
@@ -4097,8 +4346,11 @@
       <c r="G77" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>303</v>
       </c>
@@ -4121,8 +4373,11 @@
       <c r="G78" s="3" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>307</v>
       </c>
@@ -4145,8 +4400,11 @@
       <c r="G79" s="3" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>311</v>
       </c>
@@ -4169,8 +4427,11 @@
       <c r="G80" s="3" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>315</v>
       </c>
@@ -4193,8 +4454,11 @@
       <c r="G81" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>317</v>
       </c>
@@ -4217,8 +4481,11 @@
       <c r="G82" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>320</v>
       </c>
@@ -4241,8 +4508,11 @@
       <c r="G83" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>323</v>
       </c>
@@ -4265,8 +4535,11 @@
       <c r="G84" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>327</v>
       </c>
@@ -4289,8 +4562,11 @@
       <c r="G85" s="3" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>330</v>
       </c>
@@ -4308,13 +4584,16 @@
         <v>Non-Life Division</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="G86" s="3" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>331</v>
       </c>
@@ -4337,8 +4616,11 @@
       <c r="G87" s="3" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="27.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>334</v>
       </c>
@@ -4361,8 +4643,11 @@
       <c r="G88" s="3" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>339</v>
       </c>
@@ -4385,8 +4670,11 @@
       <c r="G89" s="3" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>343</v>
       </c>
@@ -4409,8 +4697,11 @@
       <c r="G90" s="3" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>345</v>
       </c>
@@ -4433,8 +4724,11 @@
       <c r="G91" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>347</v>
       </c>
@@ -4457,8 +4751,11 @@
       <c r="G92" s="3" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>353</v>
       </c>
@@ -4481,8 +4778,11 @@
       <c r="G93" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>357</v>
       </c>
@@ -4505,8 +4805,11 @@
       <c r="G94" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>361</v>
       </c>
@@ -4529,8 +4832,11 @@
       <c r="G95" s="3" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>365</v>
       </c>
@@ -4553,8 +4859,11 @@
       <c r="G96" s="3" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>369</v>
       </c>
@@ -4577,8 +4886,11 @@
       <c r="G97" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>373</v>
       </c>
@@ -4601,8 +4913,11 @@
       <c r="G98" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>377</v>
       </c>
@@ -4625,8 +4940,11 @@
       <c r="G99" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>378</v>
       </c>
@@ -4649,8 +4967,11 @@
       <c r="G100" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>380</v>
       </c>
@@ -4673,8 +4994,11 @@
       <c r="G101" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>383</v>
       </c>
@@ -4697,8 +5021,11 @@
       <c r="G102" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>385</v>
       </c>
@@ -4721,8 +5048,11 @@
       <c r="G103" s="3" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>388</v>
       </c>
@@ -4745,8 +5075,11 @@
       <c r="G104" s="3" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>391</v>
       </c>
@@ -4769,8 +5102,11 @@
       <c r="G105" s="3" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>398</v>
       </c>
@@ -4793,8 +5129,11 @@
       <c r="G106" s="3" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>401</v>
       </c>
@@ -4817,8 +5156,11 @@
       <c r="G107" s="3" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>402</v>
       </c>
@@ -4841,8 +5183,11 @@
       <c r="G108" s="3" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>405</v>
       </c>
@@ -4865,8 +5210,11 @@
       <c r="G109" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>409</v>
       </c>
@@ -4889,8 +5237,11 @@
       <c r="G110" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>412</v>
       </c>
@@ -4913,8 +5264,11 @@
       <c r="G111" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>416</v>
       </c>
@@ -4937,8 +5291,11 @@
       <c r="G112" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>420</v>
       </c>
@@ -4961,8 +5318,11 @@
       <c r="G113" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>424</v>
       </c>
@@ -4985,8 +5345,11 @@
       <c r="G114" s="3" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>427</v>
       </c>
@@ -5009,8 +5372,11 @@
       <c r="G115" s="3" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>428</v>
       </c>
@@ -5033,8 +5399,11 @@
       <c r="G116" s="3" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>429</v>
       </c>
@@ -5047,18 +5416,20 @@
       <c r="D117" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="E117" s="3" t="str">
-        <f t="array" ref="E117">INDEX(Sheet2!$C:$C,MATCH(Sheet1!F117,Sheet2!$D:$D,0))</f>
-        <v>Non-Life Division</v>
+      <c r="E117" s="3" t="s">
+        <v>507</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>432</v>
       </c>
@@ -5081,8 +5452,11 @@
       <c r="G118" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>435</v>
       </c>
@@ -5105,8 +5479,11 @@
       <c r="G119" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>437</v>
       </c>
@@ -5129,8 +5506,11 @@
       <c r="G120" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>441</v>
       </c>
@@ -5153,8 +5533,11 @@
       <c r="G121" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>445</v>
       </c>
@@ -5177,8 +5560,11 @@
       <c r="G122" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>449</v>
       </c>
@@ -5201,8 +5587,11 @@
       <c r="G123" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>453</v>
       </c>
@@ -5225,8 +5614,11 @@
       <c r="G124" s="3" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>456</v>
       </c>
@@ -5249,8 +5641,11 @@
       <c r="G125" s="3" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>460</v>
       </c>
@@ -5273,8 +5668,11 @@
       <c r="G126" s="3" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>464</v>
       </c>
@@ -5297,8 +5695,11 @@
       <c r="G127" s="3" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>468</v>
       </c>
@@ -5321,8 +5722,11 @@
       <c r="G128" s="3" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>471</v>
       </c>
@@ -5345,8 +5749,11 @@
       <c r="G129" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>474</v>
       </c>
@@ -5369,8 +5776,11 @@
       <c r="G130" s="3" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>478</v>
       </c>
@@ -5393,8 +5803,11 @@
       <c r="G131" s="3" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>482</v>
       </c>
@@ -5417,8 +5830,11 @@
       <c r="G132" s="3" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>486</v>
       </c>
@@ -5441,8 +5857,11 @@
       <c r="G133" s="3" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>490</v>
       </c>
@@ -5465,8 +5884,11 @@
       <c r="G134" s="3" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>493</v>
       </c>
@@ -5489,8 +5911,11 @@
       <c r="G135" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>497</v>
       </c>
@@ -5513,43 +5938,38 @@
       <c r="G136" s="3" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.2"/>
+      <c r="H136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="31" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="H137">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="F1:F164" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Davao Branch"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H136" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>